<commit_message>
Update db and coupler; coupler can read now the database
</commit_message>
<xml_diff>
--- a/omari_coupling.xlsx
+++ b/omari_coupling.xlsx
@@ -396,10 +396,10 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>19.02946096887985</v>
+        <v>19.3164392298743</v>
       </c>
       <c r="C2">
-        <v>0.0103782264586777</v>
+        <v>0.02882075676116136</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -407,10 +407,10 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>19.7380840709123</v>
+        <v>19.91364414806782</v>
       </c>
       <c r="C3">
-        <v>0.04631905430987032</v>
+        <v>0.04773430819931494</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -418,10 +418,10 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>18.8230242511879</v>
+        <v>19.24633245902404</v>
       </c>
       <c r="C4">
-        <v>0.02251128600002737</v>
+        <v>0.03836751660295683</v>
       </c>
     </row>
   </sheetData>

</xml_diff>